<commit_message>
Added zone creation and deletion functionality
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\netadmin\OneDrive - Ferrum High School\Desktop\CMPG323-Project4\CMPG323-Project-4---36581852\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -33,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA.csv" thousands=" " comma="1">
       <textFields count="5">
         <textField/>
@@ -45,7 +44,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(1).csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -53,7 +52,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(2).csv" thousands=" " comma="1">
       <textFields count="2">
         <textField/>
@@ -295,7 +294,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,15 +375,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(1)" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(1)" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(2)" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(2)" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,7 +682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -907,11 +906,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1036,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1124,10 +1123,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add device create and edit functionality
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\netadmin\OneDrive - Ferrum High School\Desktop\CMPG323-Project4\CMPG323-Project-4---36581852\Connected Office Web Application User Acceptance Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMPG323-Project4\CMPG323-Project-4---36581852\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="MOCK_DATA_1" localSheetId="1">Zone!$C$1:$C$201</definedName>
     <definedName name="MOCK_DATA_2" localSheetId="2">Category!$B$1:$C$196</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add zone read functionality
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMPG323-Project4\CMPG323-Project-4---36581852\Connected Office Web Application User Acceptance Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -64,221 +64,221 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="76">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>DeviceName</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>ZoneName</t>
+  </si>
   <si>
     <t>Status</t>
   </si>
   <si>
+    <t>IsActive</t>
+  </si>
+  <si>
+    <t>D01</t>
+  </si>
+  <si>
+    <t>Front-door Camera</t>
+  </si>
+  <si>
+    <t>Camera</t>
+  </si>
+  <si>
     <t>Terrazzo</t>
   </si>
   <si>
+    <t>In Operation</t>
+  </si>
+  <si>
+    <t>D02</t>
+  </si>
+  <si>
+    <t>Boiler Temp</t>
+  </si>
+  <si>
+    <t>Temperature Sensor</t>
+  </si>
+  <si>
+    <t>Boilermaker Room</t>
+  </si>
+  <si>
     <t>Broken</t>
   </si>
   <si>
+    <t>D03</t>
+  </si>
+  <si>
+    <t>Speed Testing</t>
+  </si>
+  <si>
+    <t>Speed Sensor</t>
+  </si>
+  <si>
+    <t>Safety Office</t>
+  </si>
+  <si>
+    <t>D04</t>
+  </si>
+  <si>
+    <t>Entry Access</t>
+  </si>
+  <si>
+    <t>Access Control</t>
+  </si>
+  <si>
+    <t>Stucco Mason Building</t>
+  </si>
+  <si>
+    <t>D05</t>
+  </si>
+  <si>
+    <t>Exit Access</t>
+  </si>
+  <si>
     <t>Stopped</t>
   </si>
   <si>
+    <t>D06</t>
+  </si>
+  <si>
+    <t>Light Activation</t>
+  </si>
+  <si>
+    <t>Motion Sensor</t>
+  </si>
+  <si>
+    <t>Labor Office</t>
+  </si>
+  <si>
+    <t>D07</t>
+  </si>
+  <si>
+    <t>Environmental Office</t>
+  </si>
+  <si>
+    <t>D08</t>
+  </si>
+  <si>
+    <t>Aircon Activation</t>
+  </si>
+  <si>
+    <t>Tile Setting Bench</t>
+  </si>
+  <si>
     <t>Maintenance</t>
   </si>
   <si>
+    <t>D09</t>
+  </si>
+  <si>
+    <t>Assembly Temp</t>
+  </si>
+  <si>
+    <t>Linemen Assembly</t>
+  </si>
+  <si>
+    <t>ZoneDescription</t>
+  </si>
+  <si>
+    <t>Z01</t>
+  </si>
+  <si>
     <t>13-175 - Ice Rinks</t>
   </si>
   <si>
+    <t>Z02</t>
+  </si>
+  <si>
     <t>2-870 - Sculpture/Ornamental</t>
   </si>
   <si>
+    <t>Z03</t>
+  </si>
+  <si>
     <t>17-030 - Bond</t>
   </si>
   <si>
+    <t>Z04</t>
+  </si>
+  <si>
     <t>2-750 - Concrete Pads and Walks</t>
   </si>
   <si>
+    <t>Z05</t>
+  </si>
+  <si>
+    <t>Iron Workshop</t>
+  </si>
+  <si>
     <t>3-400 - Precast Concrete</t>
   </si>
   <si>
+    <t>Z06</t>
+  </si>
+  <si>
     <t>1-523 - Sanitary Facilities</t>
   </si>
   <si>
+    <t>Z07</t>
+  </si>
+  <si>
     <t>2-370 - Erosion and Sedimentation Control</t>
   </si>
   <si>
+    <t>Z08</t>
+  </si>
+  <si>
     <t>1-570 - Temporary Controls</t>
   </si>
   <si>
+    <t>Z09</t>
+  </si>
+  <si>
     <t>2-825 - Wood Fences and Gates</t>
   </si>
   <si>
-    <t>DeviceName</t>
-  </si>
-  <si>
-    <t>CategoryName</t>
-  </si>
-  <si>
-    <t>ZoneName</t>
-  </si>
-  <si>
-    <t>IsActive</t>
-  </si>
-  <si>
-    <t>ZoneDescription</t>
-  </si>
-  <si>
     <t>CategoryDescription</t>
   </si>
   <si>
-    <t>Safety Office</t>
-  </si>
-  <si>
-    <t>Boilermaker Room</t>
-  </si>
-  <si>
-    <t>Stucco Mason Building</t>
-  </si>
-  <si>
-    <t>Iron Workshop</t>
-  </si>
-  <si>
-    <t>Labor Office</t>
-  </si>
-  <si>
-    <t>Environmental Office</t>
-  </si>
-  <si>
-    <t>Tile Setting Bench</t>
-  </si>
-  <si>
-    <t>Linemen Assembly</t>
-  </si>
-  <si>
-    <t>Camera</t>
+    <t>C01</t>
   </si>
   <si>
     <t>Visual monitoring tool</t>
   </si>
   <si>
-    <t>Temperature Sensor</t>
+    <t>C02</t>
   </si>
   <si>
     <t>Measuring air temp</t>
   </si>
   <si>
-    <t>Motion Sensor</t>
+    <t>C03</t>
   </si>
   <si>
     <t>Monitoring for motion to trigger action</t>
   </si>
   <si>
-    <t>Access Control</t>
+    <t>C04</t>
   </si>
   <si>
     <t>Managing access for people entering and exiting the zone</t>
   </si>
   <si>
-    <t>Speed Sensor</t>
+    <t>C05</t>
   </si>
   <si>
     <t>Measuring speed of moving object</t>
   </si>
   <si>
-    <t>Front-door Camera</t>
-  </si>
-  <si>
-    <t>Boiler Temp</t>
-  </si>
-  <si>
-    <t>Speed Testing</t>
-  </si>
-  <si>
-    <t>Entry Access</t>
-  </si>
-  <si>
-    <t>Exit Access</t>
-  </si>
-  <si>
-    <t>In Operation</t>
-  </si>
-  <si>
-    <t>Light Activation</t>
-  </si>
-  <si>
-    <t>Aircon Activation</t>
-  </si>
-  <si>
-    <t>Assembly Temp</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>D01</t>
-  </si>
-  <si>
-    <t>D02</t>
-  </si>
-  <si>
-    <t>D03</t>
-  </si>
-  <si>
-    <t>D04</t>
-  </si>
-  <si>
-    <t>D05</t>
-  </si>
-  <si>
-    <t>D06</t>
-  </si>
-  <si>
-    <t>D07</t>
-  </si>
-  <si>
-    <t>D08</t>
-  </si>
-  <si>
-    <t>D09</t>
-  </si>
-  <si>
-    <t>Z01</t>
-  </si>
-  <si>
-    <t>Z02</t>
-  </si>
-  <si>
-    <t>Z03</t>
-  </si>
-  <si>
-    <t>Z04</t>
-  </si>
-  <si>
-    <t>Z05</t>
-  </si>
-  <si>
-    <t>Z06</t>
-  </si>
-  <si>
-    <t>Z07</t>
-  </si>
-  <si>
-    <t>Z08</t>
-  </si>
-  <si>
-    <t>Z09</t>
-  </si>
-  <si>
-    <t>C01</t>
-  </si>
-  <si>
-    <t>C02</t>
-  </si>
-  <si>
-    <t>C03</t>
-  </si>
-  <si>
-    <t>C04</t>
-  </si>
-  <si>
-    <t>C05</t>
-  </si>
-  <si>
     <t>Create Test Passed</t>
   </si>
   <si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Delete Test Passed</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -685,12 +688,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J13:J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14 J13:J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
@@ -700,39 +704,39 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -740,19 +744,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -760,19 +764,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="b">
         <v>1</v>
@@ -780,19 +784,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="b">
         <v>1</v>
@@ -800,19 +804,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="b">
         <v>0</v>
@@ -820,19 +824,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="b">
         <v>0</v>
@@ -840,19 +844,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F8" s="2" t="b">
         <v>1</v>
@@ -860,19 +864,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F9" s="2" t="b">
         <v>0</v>
@@ -880,19 +884,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F10" s="2" t="b">
         <v>0</v>
@@ -915,118 +919,119 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1040,11 +1045,12 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection sqref="A1 A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -1052,68 +1058,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1126,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1146,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>71</v>
@@ -1157,10 +1163,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>0</v>
@@ -1174,10 +1180,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>0</v>
@@ -1191,10 +1197,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>0</v>
@@ -1208,10 +1214,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>47</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>0</v>
@@ -1225,10 +1231,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>0</v>
@@ -1242,10 +1248,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>0</v>
@@ -1259,10 +1265,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>0</v>
@@ -1276,10 +1282,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>56</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>0</v>
@@ -1293,10 +1299,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>58</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -1310,7 +1316,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>0</v>
@@ -1327,7 +1333,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>0</v>
@@ -1344,7 +1350,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2" t="b">
         <v>0</v>
@@ -1361,7 +1367,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B14" s="2" t="b">
         <v>0</v>
@@ -1378,7 +1384,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="b">
         <v>0</v>
@@ -1395,7 +1401,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="b">
         <v>0</v>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="B17" s="2" t="b">
         <v>0</v>
@@ -1429,7 +1435,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2" t="b">
         <v>0</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
@@ -1463,7 +1469,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B20" s="2" t="b">
         <v>0</v>
@@ -1480,7 +1486,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="B21" s="2" t="b">
         <v>0</v>
@@ -1497,7 +1503,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="b">
         <v>0</v>
@@ -1514,7 +1520,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="B23" s="2" t="b">
         <v>0</v>
@@ -1531,7 +1537,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B24" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Improve flowcharts and added annotations
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -289,9 +289,6 @@
   </si>
   <si>
     <t>Delete Test Passed</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1130,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,391 +1162,391 @@
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>75</v>
+      <c r="B2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>75</v>
+      <c r="B3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>75</v>
+      <c r="B4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>75</v>
+      <c r="B5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>75</v>
+      <c r="B6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>75</v>
+      <c r="B7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>75</v>
+      <c r="B8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>75</v>
+      <c r="B9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>75</v>
+      <c r="B10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>75</v>
+      <c r="B11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>75</v>
+      <c r="B12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>75</v>
+      <c r="B13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>75</v>
+      <c r="B14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>75</v>
+      <c r="B15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>75</v>
+      <c r="B16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>75</v>
+      <c r="B17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>75</v>
+      <c r="B18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>75</v>
+      <c r="B19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
+      <c r="B20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>75</v>
+      <c r="B21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>75</v>
+      <c r="B22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>75</v>
+      <c r="B23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>75</v>
+      <c r="B24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add minor changes and annotations to WriteResults.xaml
</commit_message>
<xml_diff>
--- a/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
+++ b/Connected Office Web Application User Acceptance Testing/Connected Office Test Data.xlsx
@@ -710,17 +710,17 @@
       <x:selection activeCell="J14" sqref="J14 J13:J14"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="9.109375" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="18" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="37.710938" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="37.664062" style="0" bestFit="1" customWidth="1"/>
     <x:col min="4" max="4" width="21" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="5" max="5" width="12.570312" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="6" max="6" width="8.285156" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="12.554688" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="6" max="6" width="8.332031" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -740,7 +740,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A2" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -760,7 +760,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A3" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -780,7 +780,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A4" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -800,7 +800,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A5" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -820,7 +820,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A6" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -840,7 +840,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A7" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -860,7 +860,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A8" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
@@ -880,7 +880,7 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A9" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -900,7 +900,7 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <x:c r="A10" s="2" t="s">
         <x:v>37</x:v>
       </x:c>
@@ -941,14 +941,14 @@
       <x:selection activeCell="C19" sqref="C19"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="9.109375" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="21" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="46.285156" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="46.332031" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -959,7 +959,7 @@
         <x:v>40</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A2" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
@@ -970,7 +970,7 @@
         <x:v>42</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A3" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
@@ -981,7 +981,7 @@
         <x:v>44</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A4" s="2" t="s">
         <x:v>45</x:v>
       </x:c>
@@ -992,7 +992,7 @@
         <x:v>46</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A5" s="2" t="s">
         <x:v>47</x:v>
       </x:c>
@@ -1003,7 +1003,7 @@
         <x:v>48</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A6" s="2" t="s">
         <x:v>49</x:v>
       </x:c>
@@ -1014,7 +1014,7 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A7" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
@@ -1025,7 +1025,7 @@
         <x:v>53</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A8" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
@@ -1036,7 +1036,7 @@
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A9" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -1047,7 +1047,7 @@
         <x:v>57</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <x:c r="A10" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
@@ -1079,15 +1079,15 @@
       <x:selection activeCell="A1" sqref="A1 A1:C6"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="41.285156" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="53.140625" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="11.285156" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="9.109375" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="41.332031" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="53.109375" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="11.332031" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1098,7 +1098,7 @@
         <x:v>60</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A2" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
@@ -1109,7 +1109,7 @@
         <x:v>62</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A3" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
@@ -1120,7 +1120,7 @@
         <x:v>64</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A4" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -1131,7 +1131,7 @@
         <x:v>66</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A5" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
@@ -1142,7 +1142,7 @@
         <x:v>68</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <x:c r="A6" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
@@ -1171,18 +1171,18 @@
   <x:dimension ref="A1:E24"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="K14" sqref="K14"/>
+      <x:selection activeCell="K10" sqref="K10"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <x:cols>
-    <x:col min="1" max="1" width="4.285156" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="2" max="3" width="17.855469" style="0" bestFit="1" customWidth="1"/>
-    <x:col min="4" max="4" width="18.570312" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="4.332031" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="3" width="17.886719" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="18.554688" style="0" bestFit="1" customWidth="1"/>
     <x:col min="5" max="5" width="18" style="0" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -1199,7 +1199,7 @@
         <x:v>74</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A2" s="2" t="s">
         <x:v>41</x:v>
       </x:c>
@@ -1216,7 +1216,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A3" s="2" t="s">
         <x:v>43</x:v>
       </x:c>
@@ -1233,7 +1233,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A4" s="2" t="s">
         <x:v>45</x:v>
       </x:c>
@@ -1250,7 +1250,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A5" s="2" t="s">
         <x:v>47</x:v>
       </x:c>
@@ -1267,7 +1267,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A6" s="2" t="s">
         <x:v>49</x:v>
       </x:c>
@@ -1284,7 +1284,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A7" s="2" t="s">
         <x:v>52</x:v>
       </x:c>
@@ -1301,7 +1301,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A8" s="2" t="s">
         <x:v>54</x:v>
       </x:c>
@@ -1318,7 +1318,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A9" s="2" t="s">
         <x:v>56</x:v>
       </x:c>
@@ -1335,7 +1335,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A10" s="2" t="s">
         <x:v>58</x:v>
       </x:c>
@@ -1352,7 +1352,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A11" s="2" t="s">
         <x:v>61</x:v>
       </x:c>
@@ -1369,7 +1369,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A12" s="2" t="s">
         <x:v>63</x:v>
       </x:c>
@@ -1386,7 +1386,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A13" s="2" t="s">
         <x:v>65</x:v>
       </x:c>
@@ -1403,7 +1403,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A14" s="2" t="s">
         <x:v>67</x:v>
       </x:c>
@@ -1420,7 +1420,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A15" s="2" t="s">
         <x:v>69</x:v>
       </x:c>
@@ -1437,7 +1437,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A16" s="2" t="s">
         <x:v>6</x:v>
       </x:c>
@@ -1454,7 +1454,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A17" s="2" t="s">
         <x:v>11</x:v>
       </x:c>
@@ -1471,7 +1471,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A18" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
@@ -1488,7 +1488,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A19" s="2" t="s">
         <x:v>20</x:v>
       </x:c>
@@ -1505,7 +1505,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A20" s="2" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -1522,7 +1522,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A21" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -1539,7 +1539,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A22" s="2" t="s">
         <x:v>31</x:v>
       </x:c>
@@ -1556,7 +1556,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A23" s="2" t="s">
         <x:v>33</x:v>
       </x:c>
@@ -1573,7 +1573,7 @@
         <x:v>75</x:v>
       </x:c>
     </x:row>
-    <x:row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <x:row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <x:c r="A24" s="2" t="s">
         <x:v>37</x:v>
       </x:c>

</xml_diff>